<commit_message>
update bonnes pratiques, mise en forme du tableau
</commit_message>
<xml_diff>
--- a/analyse de l'état actuel du SEO + accessibilite.xlsx
+++ b/analyse de l'état actuel du SEO + accessibilite.xlsx
@@ -74,9 +74,28 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">utiliser le format jpeg ou png</t>
-  </si>
-  <si>
+    <t xml:space="preserve">utiliser les formats standards du web , JPEG, GIF, PNG, BMP et WebP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Très lourd et long à charger, L’image se charge de bas en haut dans le navigateur,Pas de gestion de transparence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">convertir dans un format plus adapté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.oboqo.com/blog/optimiser-images-web-format-jpg-png-resolution-nom-fichier-export-photoshop/#le-format-bmp , https://support.google.com/webmasters/answer/7451184?hl=fr</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAIN</t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
@@ -85,7 +104,31 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Très lourd et long à charger, </t>
+      <t xml:space="preserve"> images trop grande</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">dimension image = dimension du contenant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l’image s’en trouve plus lourde que necessaire et allonge le temps d’affichage necessaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redimensionner les images par rapport aux contenants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAIN</t>
     </r>
     <r>
       <rPr>
@@ -93,15 +136,25 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">L’image se charge de bas en haut dans le navigateur,Pas de gestion de transparence</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">convertir dans un format plus adapté</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.oboqo.com/blog/optimiser-images-web-format-jpg-png-resolution-nom-fichier-export-photoshop/#le-format-bmp </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> images trop lourde</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">alleger au maximum les images lossy ou losseless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allonge le temps d’affichage necessaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compresser les image en lossy ou losseless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO , accessibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wave by webAIM</t>
   </si>
   <si>
     <r>
@@ -110,6 +163,7 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">MAIN</t>
     </r>
@@ -119,8 +173,36 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> texte incrusté dans des images</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">privilégier le format texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empêche un bon referencement et ne permet pas une bonne accéssibilité conformément au wcag 2 AA 1.4.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saisir le texte directement dans le html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-text-presentation.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">manuel</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Globale</t>
     </r>
     <r>
       <rPr>
@@ -130,20 +212,17 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">images trop grande</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">dimension image = dimension du contenant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l’image s’en trouve plus lourde que necessaire et allonge le temps d’affichage necessaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">redimensionner les images par rapport aux contenants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site </t>
+      <t xml:space="preserve"> css et JS non minifié</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">minifié les fichiers au maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allonge le temps d’execution des fichiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minifier les fichiers</t>
   </si>
   <si>
     <r>
@@ -152,8 +231,9 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MAIN</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Globale</t>
     </r>
     <r>
       <rPr>
@@ -161,8 +241,30 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> css et js decompressé</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">gzip les fichiers css et js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allonge le temps d’execution necessaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gzip les fichiers et ajouter le code suivant dans le .htaccess : « SetOutputFilter DEFLATE AddOutputFilterByType DEFLATE text/html text/css text/plain text/xml application/x-javascript », »BrowserMatch ^Mozilla/4 gzip-only-text/html BrowserMatch ^Mozilla/4\.0[678] no-gzip BrowserMatch \bMSIE !no-gzip !gzip-only-text/html BrowserMatch \bMSI[E] !no-gzip !gzip-only-text/html »</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Globale</t>
     </r>
     <r>
       <rPr>
@@ -172,23 +274,23 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">images trop lourde</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">alleger au maximum les images lossy ou losseless</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allonge le temps d’affichage necessaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compresser les image en lossy ou losseless</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEO , accessibilité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wave by webAIM</t>
+      <t xml:space="preserve"> vitesse d’execution scripts non optimale</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">se servire de async et defer pour les script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloquent l’affichage de la page jusqu’a ce qu’ils soient chargés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preciser si l’exécution doit etre asynchrone ou différée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aria core</t>
   </si>
   <si>
     <r>
@@ -197,8 +299,9 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MAIN</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Globale</t>
     </r>
     <r>
       <rPr>
@@ -206,178 +309,9 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">texte incrusté dans des images</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">privilégier le format texte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">empêche un bon referencement et ne permet pas une bonne accéssibilité conformément au wcag 2 AA 1.4.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">saisir le texte directement dans le html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-text-presentation.html </t>
-  </si>
-  <si>
-    <t xml:space="preserve">manuel</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Globale</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> css et JS non minifié</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">minifié les fichiers au maximum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allonge le temps d’execution des fichiers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minifier les fichiers</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Globale</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">css et js decompressé</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">gzip les fichiers css et js</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allonge le temps d’execution necessaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gzip les fichiers et ajouter le code suivant dans le .htaccess : « SetOutputFilter DEFLATE AddOutputFilterByType DEFLATE text/html text/css text/plain text/xml application/x-javascript », »BrowserMatch ^Mozilla/4 gzip-only-text/html BrowserMatch ^Mozilla/4\.0[678] no-gzip BrowserMatch \bMSIE !no-gzip !gzip-only-text/html BrowserMatch \bMSI[E] !no-gzip !gzip-only-text/html »</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Globale</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">vitesse d’execution scripts non optimale</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">se servire de async et defer pour les script</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bloquent l’affichage de la page jusqu’a ce qu’ils soient chargés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preciser si l’exécution doit etre asynchrone ou différée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accessibilité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aria core</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Globale</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Font-size &lt;12px</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Font-size &lt;12px</t>
     </r>
   </si>
   <si>
@@ -400,6 +334,7 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Globale</t>
     </r>
@@ -409,8 +344,33 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> mauvaise semantique</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre en place la semantique html5,main,section,header...etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mauvaise compréhension de la structure par les robots et la technologie d’assistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avoir un main par page et utiliser la semantique html5 (notamment « section »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://fr.semrush.com/blog/balises-structurelles-html-semantique/ </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Globale</t>
     </r>
     <r>
       <rPr>
@@ -420,20 +380,17 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">mauvaise semantique</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">mettre en place la semantique html5,main,section,header...etc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mauvaise compréhension de la structure par les robots et la technologie d’assistance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">avoir un main par page et utiliser la semantique html5 (notamment « section »</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://fr.semrush.com/blog/balises-structurelles-html-semantique/ </t>
+      <t xml:space="preserve"> pas de description</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">faire une description d’au moins 160 mots avec des keywords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mauvais referencement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages </t>
   </si>
   <si>
     <r>
@@ -442,6 +399,7 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Globale</t>
     </r>
@@ -451,8 +409,27 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> pas de title</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">title reprenant le kyword principale du site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecrire un titre reprenant le keyword principal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Globale</t>
     </r>
     <r>
       <rPr>
@@ -462,17 +439,20 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">pas de description</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">faire une description d’au moins 160 mots avec des keywords</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mauvais referencement </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages </t>
+      <t xml:space="preserve"> black hat dans les keywords meta et class</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">preferer le white hat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spam de keywords et keywords inadéquats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effacer les keywords inadéquats </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://fr.semrush.com/blog/black-hat-seo-mythe-realite/ </t>
   </si>
   <si>
     <r>
@@ -481,6 +461,7 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Globale</t>
     </r>
@@ -490,8 +471,36 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> pas de meta robots</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">placer une balise robots sur toutes les pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n’indique pas a google que l’on veut etre indexé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">placer une meta robots follow,index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578342-realisez-un-audit-de-votre-site </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeadingsMap</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAIN </t>
     </r>
     <r>
       <rPr>
@@ -501,14 +510,20 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">pas de title</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">title reprenant le kyword principale du site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecrire un titre reprenant le keyword principal</t>
+      <t xml:space="preserve">hiérarchie des niveaux de titre sémantiquement incorrecte</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">h1&gt;h2&gt;h3…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mauvaise structure du site compliquant la comprehension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">respecter une hierarchie structurellement correcte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dequeuniversity.com/rules/axe/3.5/heading-order?application=AxeChrome </t>
   </si>
   <si>
     <r>
@@ -517,8 +532,9 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Globale</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAIN </t>
     </r>
     <r>
       <rPr>
@@ -526,8 +542,33 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">pas de balises strong sur les keywords</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre les keywords en valeur pour le referencement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ne met pas les keywords en valeur pour les robots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre en valeur les keywords via les balises strong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO , accessibilité</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Globale </t>
     </r>
     <r>
       <rPr>
@@ -537,20 +578,17 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">black hat dans les keywords meta et class</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">preferer le white hat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spam de keywords et keywords inadéquats</t>
-  </si>
-  <si>
-    <t xml:space="preserve">effacer les keywords inadéquats </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://fr.semrush.com/blog/black-hat-seo-mythe-realite/ </t>
+      <t xml:space="preserve">bouton custom sans description du linking</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">toujours preciser en quoi consiste le bouton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on doit savoir a quoi correspond le bouton et ce qu’il implique ou le cas etant ou il nous mene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajouter une description</t>
   </si>
   <si>
     <r>
@@ -559,8 +597,9 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Globale</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Globale </t>
     </r>
     <r>
       <rPr>
@@ -568,8 +607,33 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">le texte alternatif du logo ne decrit pas l'image</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">emettre un texte coherent lequel decrit le contenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spam de keywords sans lien avec le logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modifier le texte alternatif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.dev/image-alt/?utm_source=lighthouse&amp;utm_medium=devtools </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MAIN </t>
     </r>
     <r>
       <rPr>
@@ -579,23 +643,14 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">pas de meta robots</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">placer une balise robots sur toutes les pages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n’indique pas a google que l’on veut etre indexé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">placer une meta robots follow,index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578342-realisez-un-audit-de-votre-site </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HeadingsMap</t>
+      <t xml:space="preserve">le texte alternatif des images ne decrit pas l'image</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">spam de keywords sans lien avec l’image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manuel et wave</t>
   </si>
   <si>
     <r>
@@ -604,6 +659,7 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">MAIN </t>
     </r>
@@ -615,20 +671,20 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">hiérarchie des niveaux de titre sémantiquement incorrecte</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">h1&gt;h2&gt;h3…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mauvaise structure du site compliquant la comprehension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">respecter une hierarchie structurellement correcte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://dequeuniversity.com/rules/axe/3.5/heading-order?application=AxeChrome </t>
+      <t xml:space="preserve">mauvais h2 (le separer en paragraphe)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ne pas mettre des paragraphes en titre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le titre englobe un ou des paragraphes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">placer le texte en tant que paragraphe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lighthouse</t>
   </si>
   <si>
     <r>
@@ -637,8 +693,9 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MAIN </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Globale </t>
     </r>
     <r>
       <rPr>
@@ -648,20 +705,17 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">pas de balises strong sur les keywords</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">mettre les keywords en valeur pour le referencement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ne met pas les keywords en valeur pour les robots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mettre en valeur les keywords via les balises strong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEO , accessibilité</t>
+      <t xml:space="preserve">linking sans description</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">toujours preciser en quoi consiste le lien et ou il va</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aucune indication sur le lien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/TR/WCAG21/ </t>
   </si>
   <si>
     <r>
@@ -670,6 +724,7 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Globale </t>
     </r>
@@ -681,17 +736,20 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">bouton custom sans description du linking</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">toujours preciser en quoi consiste le bouton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">on doit savoir a quoi correspond le bouton et ce qu’il implique ou le cas etant ou il nous mene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ajouter une description</t>
+      <t xml:space="preserve">mega annuaires dans le footer</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ne pas y avoir recours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deteriore grandement le referencement (lien de mauvaise qualité)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer les liens considérés comme mauvais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578346-augmentez-lautorite-de-votre-site </t>
   </si>
   <si>
     <r>
@@ -700,6 +758,168 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">P2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">manque de coherence avec l'accueil </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">avoir la meme presentation sur toutes les pages du contenu qui se repete (navabar, footer ….)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navbar decalée sur la droite sortant du viewport, manque de coherence avec la navbar de l’accueil</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">P2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> manque de mots dans la page pour le referencement,</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">utiliser un champs lexical varié afin de rendre le contenu interessant et d’obtenir un meilleur référencement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deteriore le referencement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer la page 2 et inclure le formulaire de contact dans la main page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibility Insights for Web </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">P2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">pas de label dans le formulaire,</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">penser accessibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formulaire non accessible par manque d’informations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajouter des informations descriptives sur les onglets du formulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/TR/UNDERSTANDING-WCAG20/ensure-compat-rsv.html </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">P2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">bouton toggle innactif,</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">avoir des boutons actifs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bouton indexé via le tab stop mais offrant aucun résultat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supprimer le bouton</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">P2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tab stops approximatifs voir erronés.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">utiliser les tab-stop sur le contenu interractif seulement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le tab stop 2 , 10 , 11 , 12 ne sont pas des éléments interactifs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modifier et simplifier le chemin de navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibility Insights for Web ,axe core</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Globale </t>
     </r>
@@ -711,20 +931,23 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">le texte alternatif du logo ne decrit pas l'image</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">emettre un texte coherent lequel decrit le contenu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spam de keywords sans lien avec le logo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modifier le texte alternatif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://web.dev/image-alt/?utm_source=lighthouse&amp;utm_medium=devtools </t>
+      <t xml:space="preserve">contraste des couleurs</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">respecter les normes wcag2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contraste constaté pas assez elevé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modifier le contraste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/Translations/NOTE-UNDERSTANDING-WCAG20-fr/visual-audio-contrast-contrast.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">axe core</t>
   </si>
   <si>
     <r>
@@ -733,8 +956,9 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MAIN </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Globale </t>
     </r>
     <r>
       <rPr>
@@ -744,14 +968,20 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">le texte alternatif des images ne decrit pas l'image</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">spam de keywords sans lien avec l’image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manuel et wave</t>
+      <t xml:space="preserve">l'attribut "lang" n'a pas une valeur valide</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">choisir un attribut valide </t>
+  </si>
+  <si>
+    <t xml:space="preserve">« defaut » n’est pas une valeur valide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lang = »fr-fr »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Attributs_universels/lang </t>
   </si>
   <si>
     <r>
@@ -760,8 +990,9 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">MAIN </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">P2</t>
     </r>
     <r>
       <rPr>
@@ -771,20 +1002,20 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">mauvais h2 (le separer en paragraphe)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ne pas mettre des paragraphes en titre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">le titre englobe un ou des paragraphes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">placer le texte en tant que paragraphe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lighthouse</t>
+      <t xml:space="preserve"> les liens n'ont pas un texte perceptible</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ne pas faire de lien fantomatique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les liens n’indiquent pas ce qu’ils sont nous ou ils vont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajouter du texte ,supprimer le lien ou modifier la couleur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dequeuniversity.com/rules/axe/3.5/link-name?application=AxeChrome </t>
   </si>
   <si>
     <r>
@@ -793,6 +1024,7 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Globale </t>
     </r>
@@ -804,17 +1036,20 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">linking sans description</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">toujours preciser en quoi consiste le lien et ou il va</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aucune indication sur le lien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.w3.org/TR/WCAG21/ </t>
+      <t xml:space="preserve">Contenu non imbriqué dans une région ARIA</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">utiliser ARIA pour l’accessibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">structure non determinée pour les technologies d’assistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre en place une semantique claire et ou des ARIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/TR/WCAG20-TECHS/ARIA11.html </t>
   </si>
   <si>
     <r>
@@ -823,8 +1058,9 @@
         <color rgb="FFC9211E"/>
         <rFont val="Arial"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Globale </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">P2 </t>
     </r>
     <r>
       <rPr>
@@ -834,20 +1070,20 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">mega annuaires dans le footer</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ne pas y avoir recours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deteriore grandement le referencement (lien de mauvaise qualité)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supprimer les liens considérés comme mauvais</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578346-augmentez-lautorite-de-votre-site </t>
+      <t xml:space="preserve">h1 transparent</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">couleur de fonts différente du background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">texte invisible pour les utilisateurs, peut etre consideré comme technique de black hat par google</t>
+  </si>
+  <si>
+    <t xml:space="preserve">détacher le texte du background contraste de 4.5:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://webaim.org/standards/wcag/checklist#sc1.4.3 </t>
   </si>
   <si>
     <r>
@@ -857,336 +1093,6 @@
         <rFont val="Arial"/>
         <family val="0"/>
         <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">P2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">manque de coherence avec l'accueil </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">avoir la meme presentation sur toutes les pages du contenu qui se repete (navabar, footer ….)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">navbar decalée sur la droite sortant du viewport, manque de coherence avec la navbar de l’accueil</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">P2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> manque de mots dans la page pour le referencement,</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">utiliser un champs lexical varié afin de rendre le contenu interessant et d’obtenir un meilleur référencement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deteriore le referencement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supprimer la page 2 et inclure le formulaire de contact dans la main page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accessibility Insights for Web </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">P2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">pas de label dans le formulaire,</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">penser accessibilité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">formulaire non accessible par manque d’informations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ajouter des informations descriptives sur les onglets du formulaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.w3.org/TR/UNDERSTANDING-WCAG20/ensure-compat-rsv.html </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">P2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">bouton toggle innactif,</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">avoir des boutons actifs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bouton indexé via le tab stop mais offrant aucun résultat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supprimer le bouton</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">P2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">tab stops approximatifs voir erronés.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">utiliser les tab-stop sur le contenu interractif seulement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">le tab stop 2 , 10 , 11 , 12 ne sont pas des éléments interactifs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modifier et simplifier le chemin de navigation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accessibility Insights for Web ,axe core</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Globale </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">contraste des couleurs</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">respecter les normes wcag2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contraste constaté pas assez elevé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modifier le contraste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.w3.org/Translations/NOTE-UNDERSTANDING-WCAG20-fr/visual-audio-contrast-contrast.html </t>
-  </si>
-  <si>
-    <t xml:space="preserve">axe core</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Globale </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">l'attribut "lang" n'a pas une valeur valide</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">choisir un attribut valide </t>
-  </si>
-  <si>
-    <t xml:space="preserve">« defaut » n’est pas une valeur valide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lang = »fr-fr »</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Attributs_universels/lang </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">P2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> les liens n'ont pas un texte perceptible</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ne pas faire de lien fantomatique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">les liens n’indiquent pas ce qu’ils sont nous ou ils vont</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ajouter du texte ,supprimer le lien ou modifier la couleur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://dequeuniversity.com/rules/axe/3.5/link-name?application=AxeChrome </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Globale </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Contenu non imbriqué dans une région ARIA</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">utiliser ARIA pour l’accessibilité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">structure non determinée pour les technologies d’assistance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mettre en place une semantique claire et ou des ARIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.w3.org/TR/WCAG20-TECHS/ARIA11.html </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">P2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">h1 transparent</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">couleur de fonts différente du background</t>
-  </si>
-  <si>
-    <t xml:space="preserve">texte invisible pour les utilisateurs, peut etre consideré comme technique de black hat par google</t>
-  </si>
-  <si>
-    <t xml:space="preserve">détacher le texte du background contraste de 4.5:1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://webaim.org/standards/wcag/checklist#sc1.4.3 </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
       </rPr>
       <t xml:space="preserve">Globale </t>
     </r>
@@ -1221,7 +1127,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1279,14 +1185,8 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFC9211E"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1299,13 +1199,50 @@
         <bgColor rgb="FF993366"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD8CE"/>
+        <bgColor rgb="FFDEE6EF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEE6EF"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA6A6"/>
+        <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -1334,7 +1271,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1351,20 +1288,60 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1392,12 +1369,12 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF7030A0"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFFFFFD7"/>
+      <rgbColor rgb="FFDEE6EF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -1415,9 +1392,9 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFFA6A6"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFD8CE"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1447,10 +1424,10 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.67"/>
@@ -1458,7 +1435,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="43.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="8" style="0" width="10.56"/>
   </cols>
   <sheetData>
@@ -1509,733 +1486,788 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="31.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="10"/>
+    </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" customFormat="false" ht="124.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" customFormat="false" ht="28.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="48.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" s="10" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" customFormat="false" ht="31.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" customFormat="false" ht="31.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="B18" s="11"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" customFormat="false" ht="33.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" customFormat="false" ht="33.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="15" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" customFormat="false" ht="31.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" customFormat="false" ht="31.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" s="15" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" customFormat="false" ht="32.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" customFormat="false" ht="31.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F27" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" customFormat="false" ht="46.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="14" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="F30" s="15"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" customFormat="false" ht="46.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="F31" s="15" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" customFormat="false" ht="32.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="F32" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" customFormat="false" ht="32.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="F33" s="0" t="s">
+      <c r="F33" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" customFormat="false" ht="31.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="F34" s="15" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" customFormat="false" ht="32.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="F35" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G35" s="10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" customFormat="false" ht="32.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="F36" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G36" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" customFormat="false" ht="31.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="F37" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="G37" s="10" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" customFormat="false" ht="30.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="F38" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G38" s="10" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" customFormat="false" ht="33.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="F39" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="G39" s="10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" customFormat="false" ht="31.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="F40" s="0" t="s">
+      <c r="F40" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="G40" s="10" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3201,32 +3233,31 @@
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" location="le-format-bmp" display="https://www.oboqo.com/blog/optimiser-images-web-format-jpg-png-resolution-nom-fichier-export-photoshop/#le-format-bmp"/>
-    <hyperlink ref="G4" r:id="rId2" display="https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site"/>
-    <hyperlink ref="G5" r:id="rId3" display="https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site"/>
-    <hyperlink ref="G6" r:id="rId4" display="https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-text-presentation.html"/>
-    <hyperlink ref="G8" r:id="rId5" display="https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site"/>
-    <hyperlink ref="G9" r:id="rId6" display="https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site"/>
-    <hyperlink ref="G10" r:id="rId7" display="https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site"/>
-    <hyperlink ref="G12" r:id="rId8" display="https://medium.muz.li/typography-in-mobile-design-15-best-practices-to-excellent-ui-5eaf18280ad"/>
-    <hyperlink ref="G14" r:id="rId9" display="https://fr.semrush.com/blog/balises-structurelles-html-semantique/"/>
-    <hyperlink ref="G15" r:id="rId10" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages"/>
-    <hyperlink ref="G16" r:id="rId11" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages"/>
-    <hyperlink ref="G17" r:id="rId12" display="https://fr.semrush.com/blog/black-hat-seo-mythe-realite/"/>
-    <hyperlink ref="G19" r:id="rId13" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578342-realisez-un-audit-de-votre-site"/>
-    <hyperlink ref="G20" r:id="rId14" display="https://dequeuniversity.com/rules/axe/3.5/heading-order?application=AxeChrome"/>
-    <hyperlink ref="G23" r:id="rId15" display="https://web.dev/image-alt/?utm_source=lighthouse&amp;utm_medium=devtools"/>
-    <hyperlink ref="G24" r:id="rId16" display="https://web.dev/image-alt/?utm_source=lighthouse&amp;utm_medium=devtools"/>
-    <hyperlink ref="G26" r:id="rId17" display="https://www.w3.org/TR/WCAG21/"/>
-    <hyperlink ref="G27" r:id="rId18" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578346-augmentez-lautorite-de-votre-site"/>
-    <hyperlink ref="G32" r:id="rId19" display="https://www.w3.org/TR/UNDERSTANDING-WCAG20/ensure-compat-rsv.html"/>
-    <hyperlink ref="G33" r:id="rId20" display="https://www.w3.org/TR/WCAG21/"/>
-    <hyperlink ref="G35" r:id="rId21" display="https://www.w3.org/Translations/NOTE-UNDERSTANDING-WCAG20-fr/visual-audio-contrast-contrast.html"/>
-    <hyperlink ref="G36" r:id="rId22" display="https://developer.mozilla.org/fr/docs/Web/HTML/Attributs_universels/lang"/>
-    <hyperlink ref="G37" r:id="rId23" display="https://dequeuniversity.com/rules/axe/3.5/link-name?application=AxeChrome"/>
-    <hyperlink ref="G38" r:id="rId24" display="https://www.w3.org/TR/WCAG20-TECHS/ARIA11.html"/>
-    <hyperlink ref="G39" r:id="rId25" location="sc1.4.3" display="https://webaim.org/standards/wcag/checklist#sc1.4.3"/>
-    <hyperlink ref="G40" r:id="rId26" location="sc2.4.4" display="https://webaim.org/standards/wcag/checklist#sc2.4.4"/>
+    <hyperlink ref="G4" r:id="rId1" display="https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site "/>
+    <hyperlink ref="G5" r:id="rId2" display="https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site "/>
+    <hyperlink ref="G6" r:id="rId3" display="https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-text-presentation.html "/>
+    <hyperlink ref="G8" r:id="rId4" display="https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site "/>
+    <hyperlink ref="G9" r:id="rId5" display="https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site "/>
+    <hyperlink ref="G10" r:id="rId6" display="https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site "/>
+    <hyperlink ref="G12" r:id="rId7" display="https://medium.muz.li/typography-in-mobile-design-15-best-practices-to-excellent-ui-5eaf18280ad"/>
+    <hyperlink ref="G14" r:id="rId8" display="https://fr.semrush.com/blog/balises-structurelles-html-semantique/ "/>
+    <hyperlink ref="G15" r:id="rId9" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages "/>
+    <hyperlink ref="G16" r:id="rId10" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages "/>
+    <hyperlink ref="G17" r:id="rId11" display="https://fr.semrush.com/blog/black-hat-seo-mythe-realite/ "/>
+    <hyperlink ref="G19" r:id="rId12" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578342-realisez-un-audit-de-votre-site "/>
+    <hyperlink ref="G20" r:id="rId13" display="https://dequeuniversity.com/rules/axe/3.5/heading-order?application=AxeChrome "/>
+    <hyperlink ref="G23" r:id="rId14" display="https://web.dev/image-alt/?utm_source=lighthouse&amp;utm_medium=devtools "/>
+    <hyperlink ref="G24" r:id="rId15" display="https://web.dev/image-alt/?utm_source=lighthouse&amp;utm_medium=devtools "/>
+    <hyperlink ref="G26" r:id="rId16" display="https://www.w3.org/TR/WCAG21/ "/>
+    <hyperlink ref="G27" r:id="rId17" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578346-augmentez-lautorite-de-votre-site "/>
+    <hyperlink ref="G32" r:id="rId18" display="https://www.w3.org/TR/UNDERSTANDING-WCAG20/ensure-compat-rsv.html "/>
+    <hyperlink ref="G33" r:id="rId19" display="https://www.w3.org/TR/WCAG21/ "/>
+    <hyperlink ref="G35" r:id="rId20" display="https://www.w3.org/Translations/NOTE-UNDERSTANDING-WCAG20-fr/visual-audio-contrast-contrast.html "/>
+    <hyperlink ref="G36" r:id="rId21" display="https://developer.mozilla.org/fr/docs/Web/HTML/Attributs_universels/lang "/>
+    <hyperlink ref="G37" r:id="rId22" display="https://dequeuniversity.com/rules/axe/3.5/link-name?application=AxeChrome "/>
+    <hyperlink ref="G38" r:id="rId23" display="https://www.w3.org/TR/WCAG20-TECHS/ARIA11.html "/>
+    <hyperlink ref="G39" r:id="rId24" location="sc1.4.3" display="https://webaim.org/standards/wcag/checklist#sc1.4.3 "/>
+    <hyperlink ref="G40" r:id="rId25" location="sc2.4.4" display="https://webaim.org/standards/wcag/checklist#sc2.4.4 "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>